<commit_message>
Add upload function to controller
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>salary</t>
   </si>
   <si>
     <t>francisco</t>
@@ -60,10 +63,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -81,6 +84,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -89,6 +98,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -97,14 +114,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -112,44 +153,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,14 +174,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -188,6 +191,13 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,30 +213,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,13 +243,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,169 +393,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,40 +438,27 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,21 +487,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -522,173 +496,204 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1010,20 +1015,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="17.2857142857143" customWidth="1"/>
     <col min="3" max="3" width="23.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="11.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" spans="1:3">
+    <row r="1" ht="19.5" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1033,60 +1039,78 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5000.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2500</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>